<commit_message>
Updated and ready to send to Graphic Artist
</commit_message>
<xml_diff>
--- a/Copy/2018-Fall/word count.xlsx
+++ b/Copy/2018-Fall/word count.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18940" windowHeight="11340" tabRatio="291"/>
+    <workbookView xWindow="2700" yWindow="140" windowWidth="18940" windowHeight="11340" tabRatio="291"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="A5" authorId="0">
+    <comment ref="A8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>Article</t>
   </si>
@@ -64,12 +64,6 @@
     <t>Actual Delivered</t>
   </si>
   <si>
-    <t>Cowboy Festival</t>
-  </si>
-  <si>
-    <t>Alex Gooch</t>
-  </si>
-  <si>
     <t>Critters</t>
   </si>
   <si>
@@ -88,15 +82,6 @@
     <t>Margi Bertram</t>
   </si>
   <si>
-    <t>Hittin' the Trail</t>
-  </si>
-  <si>
-    <t>Bill Miller</t>
-  </si>
-  <si>
-    <t>Cowboy Festival Flyer</t>
-  </si>
-  <si>
     <t>Back Page</t>
   </si>
   <si>
@@ -113,6 +98,39 @@
   </si>
   <si>
     <t>Pages:</t>
+  </si>
+  <si>
+    <t>Silents</t>
+  </si>
+  <si>
+    <t>Bill Blowers</t>
+  </si>
+  <si>
+    <t>Pow Wow &amp; other Flyers</t>
+  </si>
+  <si>
+    <t>Bob Hoke</t>
+  </si>
+  <si>
+    <t>Meet a board member</t>
+  </si>
+  <si>
+    <t>Tim Murphy</t>
+  </si>
+  <si>
+    <t>Goin Country</t>
+  </si>
+  <si>
+    <t>Hart Books</t>
+  </si>
+  <si>
+    <t>Jennie????</t>
+  </si>
+  <si>
+    <t>Hart's Other Home</t>
+  </si>
+  <si>
+    <t>Bill West</t>
   </si>
 </sst>
 </file>
@@ -205,7 +223,7 @@
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>584200</xdr:colOff>
-      <xdr:row>80</xdr:row>
+      <xdr:row>83</xdr:row>
       <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -571,10 +589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -615,218 +633,283 @@
     </row>
     <row r="2" spans="1:9" ht="15">
       <c r="A2" s="3" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C2" s="3">
-        <v>529</v>
+        <v>500</v>
       </c>
       <c r="D2" s="3">
         <v>1</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3">
-        <v>529</v>
+        <v>448</v>
       </c>
       <c r="G2" s="3">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15">
       <c r="A3" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3" s="3">
-        <v>194</v>
+        <v>500</v>
       </c>
       <c r="D3" s="3">
         <v>3</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3">
-        <v>194</v>
+        <v>520</v>
       </c>
       <c r="G3" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15">
       <c r="A4" s="3" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="3">
-        <v>222</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="C4" s="3"/>
       <c r="D4" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3">
-        <v>222</v>
+        <v>14</v>
       </c>
       <c r="G4" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15">
       <c r="A5" s="3" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="C5" s="3">
         <v>500</v>
       </c>
       <c r="D5" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3">
-        <v>0</v>
+        <v>479</v>
       </c>
       <c r="G5" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15">
       <c r="A6" s="3" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="C6" s="3">
-        <v>1200</v>
+        <v>200</v>
       </c>
       <c r="D6" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3">
-        <v>1200</v>
+        <v>106</v>
       </c>
       <c r="G6" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15">
       <c r="A7" s="3" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C7" s="3">
-        <v>600</v>
-      </c>
-      <c r="D7" s="3"/>
+        <v>500</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1</v>
+      </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3">
-        <v>600</v>
-      </c>
-      <c r="G7" s="3"/>
+        <v>222</v>
+      </c>
+      <c r="G7" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:9" ht="15">
       <c r="A8" s="3" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C8" s="3">
-        <v>600</v>
+        <v>500</v>
       </c>
       <c r="D8" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3">
+        <v>146</v>
+      </c>
+      <c r="G8" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15">
+      <c r="A9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="3">
+        <v>500</v>
+      </c>
+      <c r="D9" s="3">
+        <v>2</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3">
+        <v>550</v>
+      </c>
+      <c r="G9" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15">
+      <c r="A10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="3">
         <v>600</v>
       </c>
-      <c r="G8" s="3"/>
-    </row>
-    <row r="9" spans="1:9" ht="15">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-    </row>
-    <row r="10" spans="1:9" ht="15">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
+      <c r="D10" s="3">
+        <v>2</v>
+      </c>
       <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
+      <c r="F10" s="3">
+        <v>600</v>
+      </c>
+      <c r="G10" s="3">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:9" ht="15">
-      <c r="A11" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="5">
-        <f>SUM(C2:C10)</f>
-        <v>3845</v>
-      </c>
-      <c r="D11" s="5">
-        <f>SUM(D2:D10)</f>
-        <v>8</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" s="5">
-        <f>SUM(F2:F10)</f>
-        <v>3345</v>
-      </c>
-      <c r="G11" s="5">
-        <f>SUM(G2:G10)</f>
-        <v>8</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>21</v>
-      </c>
+      <c r="A11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="3">
+        <v>600</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3">
+        <v>600</v>
+      </c>
+      <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:9" ht="15">
       <c r="A12" s="3"/>
-      <c r="B12" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="7">
-        <f>C11/600</f>
-        <v>6.4083333333333332</v>
-      </c>
-      <c r="D12" s="7">
-        <f>D11/5</f>
-        <v>1.6</v>
-      </c>
-      <c r="E12" s="7">
-        <f>SUM(C12:D12)</f>
-        <v>8.0083333333333329</v>
-      </c>
-      <c r="F12" s="7">
-        <f>F11/600</f>
-        <v>5.5750000000000002</v>
-      </c>
-      <c r="G12" s="7">
-        <f>G11/5</f>
-        <v>1.6</v>
-      </c>
-      <c r="H12" s="8">
-        <f>SUM(F12:G12)</f>
-        <v>7.1750000000000007</v>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="1:9" ht="15">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="1:9" ht="15">
+      <c r="A14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="5">
+        <f>SUM(C2:C13)</f>
+        <v>4400</v>
+      </c>
+      <c r="D14" s="5">
+        <f>SUM(D2:D13)</f>
+        <v>17</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="5">
+        <f>SUM(F2:F13)</f>
+        <v>3685</v>
+      </c>
+      <c r="G14" s="5">
+        <f>SUM(G2:G13)</f>
+        <v>27</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15">
+      <c r="A15" s="3"/>
+      <c r="B15" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="7">
+        <f>C14/600</f>
+        <v>7.333333333333333</v>
+      </c>
+      <c r="D15" s="7">
+        <f>D14/5</f>
+        <v>3.4</v>
+      </c>
+      <c r="E15" s="7">
+        <f>SUM(C15:D15)</f>
+        <v>10.733333333333333</v>
+      </c>
+      <c r="F15" s="7">
+        <f>F14/600</f>
+        <v>6.1416666666666666</v>
+      </c>
+      <c r="G15" s="7">
+        <f>G14/5</f>
+        <v>5.4</v>
+      </c>
+      <c r="H15" s="8">
+        <f>SUM(F15:G15)</f>
+        <v>11.541666666666668</v>
       </c>
     </row>
   </sheetData>

</xml_diff>